<commit_message>
* Se libera version 1.04 de PLC y 1.3.0 de PC
</commit_message>
<xml_diff>
--- a/Programas/estructura paso.xlsx
+++ b/Programas/estructura paso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\lavadora.net\Programas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648D3578-EEA2-4F0D-A09E-CC4963E85D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3D6E44-2358-4C99-A4A9-8114630EEA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Paso</t>
   </si>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>Plantilla</t>
-  </si>
-  <si>
-    <t>MeterAditIzq</t>
-  </si>
-  <si>
-    <t>MeterAditDer</t>
   </si>
   <si>
     <t>FUNCION</t>
@@ -273,11 +267,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,7 +688,7 @@
   <dimension ref="A2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="111" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -703,18 +697,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -750,12 +744,12 @@
     </row>
     <row r="4" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
@@ -801,12 +795,12 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="9" t="s">
@@ -820,11 +814,11 @@
       <c r="A8" s="2">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="1"/>
       <c r="G8" s="3" t="s">
         <v>40</v>
@@ -836,21 +830,21 @@
         <v>42</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="e">
@@ -866,11 +860,11 @@
       <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="G10" s="2" t="s">
         <v>23</v>
@@ -891,11 +885,11 @@
       <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="1"/>
       <c r="G11" s="2" t="s">
         <v>25</v>
@@ -916,11 +910,11 @@
       <c r="A12" s="2">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="G12" s="2" t="s">
         <v>27</v>
@@ -941,11 +935,11 @@
       <c r="A13" s="2">
         <v>5</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="1"/>
       <c r="G13" s="2" t="s">
         <v>29</v>
@@ -966,14 +960,14 @@
       <c r="A14" s="2">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>38</v>
@@ -991,11 +985,11 @@
       <c r="A15" s="2">
         <v>7</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="1"/>
       <c r="G15" s="2" t="s">
         <v>30</v>
@@ -1016,11 +1010,11 @@
       <c r="A16" s="2">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="G16" s="2" t="s">
         <v>31</v>
@@ -1041,11 +1035,11 @@
       <c r="A17" s="2">
         <v>9</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2" t="s">
@@ -1067,11 +1061,9 @@
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="2" t="s">
@@ -1093,16 +1085,14 @@
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
       <c r="H19" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1117,11 +1107,11 @@
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
@@ -1139,9 +1129,9 @@
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1153,9 +1143,9 @@
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1167,9 +1157,9 @@
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1179,12 +1169,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
@@ -1193,11 +1182,12 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
@@ -1220,7 +1210,7 @@
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">

</xml_diff>